<commit_message>
corrected stellar parameters retrieval
</commit_message>
<xml_diff>
--- a/results/consolidated_HD_results.xlsx
+++ b/results/consolidated_HD_results.xlsx
@@ -434,7 +434,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="21" customWidth="1" min="1" max="1"/>
+    <col width="30" customWidth="1" min="1" max="1"/>
     <col width="21" customWidth="1" min="2" max="2"/>
     <col width="21" customWidth="1" min="3" max="3"/>
     <col width="19" customWidth="1" min="4" max="4"/>
@@ -561,7 +561,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>100254161710940928</t>
+          <t>Gaia DR3 100254161710940928</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -636,7 +636,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>100380639907919872</t>
+          <t>Gaia DR3 100380639907919872</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -711,7 +711,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>100586763978318208</t>
+          <t>Gaia DR3 100586763978318208</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -773,7 +773,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>100665065526715008</t>
+          <t>Gaia DR3 100665065526715008</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -821,7 +821,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>101283987497967360</t>
+          <t>Gaia DR3 101283987497967360</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -888,7 +888,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>101309452355657216</t>
+          <t>Gaia DR3 101309452355657216</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>101489256866566528</t>
+          <t>Gaia DR3 101489256866566528</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1020,7 +1020,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>101612981989146752</t>
+          <t>Gaia DR3 101612981989146752</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1073,7 +1073,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>102082409030066560</t>
+          <t>Gaia DR3 102082409030066560</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>102082477749475200</t>
+          <t>Gaia DR3 102082477749475200</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1223,7 +1223,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>102162639019033600</t>
+          <t>Gaia DR3 102162639019033600</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1290,7 +1290,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>102648588798884736</t>
+          <t>Gaia DR3 102648588798884736</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1355,7 +1355,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>103124230657005568</t>
+          <t>Gaia DR3 103124230657005568</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1417,7 +1417,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>103173223348678144</t>
+          <t>Gaia DR3 103173223348678144</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1479,7 +1479,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>103363168277756928</t>
+          <t>Gaia DR3 103363168277756928</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1546,7 +1546,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>103649316178540416</t>
+          <t>Gaia DR3 103649316178540416</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1616,7 +1616,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>103942679624729088</t>
+          <t>Gaia DR3 103942679624729088</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1681,7 +1681,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>104453918172129792</t>
+          <t>Gaia DR3 104453918172129792</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1756,7 +1756,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>104716907609412352</t>
+          <t>Gaia DR3 104716907609412352</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1820,7 +1820,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>104717285566534016</t>
+          <t>Gaia DR3 104717285566534016</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1890,7 +1890,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>104752950974981760</t>
+          <t>Gaia DR2 104752950974981760</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1942,7 +1942,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>105332908999068032</t>
+          <t>Gaia DR3 105332908999068032</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2017,7 +2017,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>105599987244856064</t>
+          <t>Gaia DR2 105599987244856064</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2057,7 +2057,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>10584899657116672</t>
+          <t>Gaia DR3 10584899657116672</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2132,7 +2132,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>105850121845012608</t>
+          <t>Gaia DR3 105850121845012608</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2180,7 +2180,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>106051542927008128</t>
+          <t>Gaia DR3 106051542927008128</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2255,7 +2255,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>10608573516849536</t>
+          <t>Gaia DR3 10608573516849536</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2330,7 +2330,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>106774952858617088</t>
+          <t>Gaia DR3 106774952858617088</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2405,7 +2405,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>107175480033033472</t>
+          <t>Gaia DR3 107175480033033472</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2467,7 +2467,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>107774198474602368</t>
+          <t>Gaia DR3 107774198474602368</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -2542,7 +2542,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>107774202769886848</t>
+          <t>Gaia DR3 107774202769886848</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2617,7 +2617,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>108421608959951488</t>
+          <t>Gaia DR3 108421608959951488</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2682,7 +2682,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>109051246870008448</t>
+          <t>Gaia DR3 109051246870008448</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2752,7 +2752,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>109628013733250304</t>
+          <t>Gaia DR3 109628013733250304</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -2814,7 +2814,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>109931856900594432</t>
+          <t>Gaia DR3 109931856900594432</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -2889,7 +2889,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>11037726649058432</t>
+          <t>Gaia DR3 11037726649058432</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -2956,7 +2956,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>111379432679196672</t>
+          <t>Gaia DR3 111379432679196672</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3028,7 +3028,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>11210418694164864</t>
+          <t>Gaia DR2 11210418694164864</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>112440873718983680</t>
+          <t>Gaia DR3 112440873718983680</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -3163,7 +3163,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>114207651462714880</t>
+          <t>Gaia DR3 114207651462714880</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3235,7 +3235,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>114575472461716864</t>
+          <t>Gaia DR3 114575472461716864</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3315,7 +3315,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>114832620743735808</t>
+          <t>Gaia DR3 114832620743735808</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3395,7 +3395,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>11530342218200448</t>
+          <t>Gaia DR3 11530342218200448</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -3433,7 +3433,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>115311458058061440</t>
+          <t>Gaia DR3 115311458058061440</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3513,7 +3513,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>1153462739205798528</t>
+          <t>Gaia DR3 1153462739205798528</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3567,7 +3567,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>115364234616059392</t>
+          <t>Gaia DR3 115364234616059392</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3642,7 +3642,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>1154336202410495488</t>
+          <t>Gaia DR3 1154336202410495488</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -3717,7 +3717,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>1154866579332084992</t>
+          <t>Gaia DR3 1154866579332084992</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -3765,7 +3765,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>1155276250492687616</t>
+          <t>Gaia DR3 1155276250492687616</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -3837,7 +3837,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>1156350542072311936</t>
+          <t>Gaia DR3 1156350542072311936</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -3880,7 +3880,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>1156846524895814144</t>
+          <t>Gaia DR3 1156846524895814144</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -3947,7 +3947,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>1157670986817726976</t>
+          <t>Gaia DR3 1157670986817726976</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4012,7 +4012,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>1157737335472646016</t>
+          <t>Gaia DR3 1157737335472646016</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4087,7 +4087,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>1158184012071254400</t>
+          <t>Gaia DR2 1158184012071254400</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4144,7 +4144,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>1158503591997923072</t>
+          <t>Gaia DR3 1158503591997923072</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4209,7 +4209,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>1159380486880813952</t>
+          <t>Gaia DR3 1159380486880813952</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -4261,7 +4261,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>1159502154714284544</t>
+          <t>Gaia DR3 1159502154714284544</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -4318,7 +4318,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>1159502498311670144</t>
+          <t>Gaia DR3 1159502498311670144</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -4388,7 +4388,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>1159605302648975104</t>
+          <t>Gaia DR3 1159605302648975104</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -4468,7 +4468,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>1159745146784043264</t>
+          <t>Gaia DR3 1159745146784043264</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -4535,7 +4535,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>1160184436039120128</t>
+          <t>Gaia DR3 1160184436039120128</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -4599,7 +4599,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>116037204451525376</t>
+          <t>Gaia DR3 116037204451525376</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -4679,7 +4679,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>116037371954842240</t>
+          <t>Gaia DR3 116037371954842240</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -4746,7 +4746,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>1160612111702571776</t>
+          <t>Gaia DR3 1160612111702571776</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -4799,7 +4799,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>1160716496587849088</t>
+          <t>Gaia DR3 1160716496587849088</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -4861,7 +4861,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>1160956465000504448</t>
+          <t>Gaia DR3 1160956465000504448</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -4936,7 +4936,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>1161042158187967232</t>
+          <t>Gaia DR3 1161042158187967232</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -4989,7 +4989,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>1161759314647344896</t>
+          <t>Gaia DR3 1161759314647344896</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -5064,7 +5064,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>1161797900633510144</t>
+          <t>Gaia DR3 1161797900633510144</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -5139,7 +5139,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>116261779701601152</t>
+          <t>Gaia DR3 116261779701601152</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -5211,7 +5211,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>1162946718486550272</t>
+          <t>Gaia DR3 1162946718486550272</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -5273,7 +5273,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>1163192665493054336</t>
+          <t>Gaia DR3 1163192665493054336</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -5338,7 +5338,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>116339982465090048</t>
+          <t>Gaia DR2 116339982465090048</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -5395,7 +5395,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>1163549697534289664</t>
+          <t>Gaia DR3 1163549697534289664</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -5470,7 +5470,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>1164145048721331968</t>
+          <t>Gaia DR3 1164145048721331968</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -5527,7 +5527,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>116456668137575040</t>
+          <t>Gaia DR3 116456668137575040</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -5580,7 +5580,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>1165262633571848064</t>
+          <t>Gaia DR3 1165262633571848064</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -5655,7 +5655,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>1165859359148269568</t>
+          <t>Gaia DR3 1165859359148269568</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -5730,7 +5730,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>1166203712446038912</t>
+          <t>Gaia DR3 1166203712446038912</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -5778,7 +5778,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>1166216253750406144</t>
+          <t>Gaia DR3 1166216253750406144</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -5853,7 +5853,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>1166577855636534144</t>
+          <t>Gaia DR3 1166577855636534144</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -5915,7 +5915,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>1167718049194619136</t>
+          <t>Gaia DR3 1167718049194619136</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -5985,7 +5985,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>1167718049194619264</t>
+          <t>Gaia DR3 1167718049194619264</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -6055,7 +6055,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>1167838720595878400</t>
+          <t>Gaia DR3 1167838720595878400</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -6125,7 +6125,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>1168984617870183808</t>
+          <t>Gaia DR3 1168984617870183808</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -6185,7 +6185,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>1169984108299812608</t>
+          <t>Gaia DR3 1169984108299812608</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -6250,7 +6250,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>1170092547633728256</t>
+          <t>Gaia DR3 1170092547633728256</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -6298,7 +6298,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>1170098251350303616</t>
+          <t>Gaia DR2 1170098251350303616</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -6339,7 +6339,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>1170359243627867904</t>
+          <t>Gaia DR3 1170359243627867904</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -6401,7 +6401,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>1170797781264303616</t>
+          <t>Gaia DR3 1170797781264303616</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -6476,7 +6476,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>1171453979251962624</t>
+          <t>Gaia DR3 1171453979251962624</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -6524,7 +6524,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>1171574685013520640</t>
+          <t>Gaia DR3 1171574685013520640</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -6594,7 +6594,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>1172340086840027264</t>
+          <t>Gaia DR2 1172340086840027264</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -6646,7 +6646,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>1173206811240350592</t>
+          <t>Gaia DR3 1173206811240350592</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -6711,7 +6711,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>1173847139324624256</t>
+          <t>Gaia DR3 1173847139324624256</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -6776,7 +6776,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>1173992103060678272</t>
+          <t>Gaia DR3 1173992103060678272</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -6841,7 +6841,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>1174143182830505856</t>
+          <t>Gaia DR3 1174143182830505856</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -6894,7 +6894,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>1174143182830505984</t>
+          <t>Gaia DR3 1174143182830505984</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -6974,7 +6974,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>1174189362318863488</t>
+          <t>Gaia DR3 1174189362318863488</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -7041,7 +7041,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>1174513645233715584</t>
+          <t>Gaia DR3 1174513645233715584</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">

</xml_diff>